<commit_message>
Added Queue Module, POM and CommonStep
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -5,6 +5,9 @@
   <sheets>
     <sheet state="visible" name="Browser" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Register" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Queue" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Tree" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="CodeEditor" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>Browser</t>
   </si>
@@ -35,15 +38,15 @@
     <t>https://dsportalapp.herokuapp.com/home</t>
   </si>
   <si>
+    <t>abc@tester.com</t>
+  </si>
+  <si>
+    <t>testtest@1</t>
+  </si>
+  <si>
     <t>abc@test.com</t>
   </si>
   <si>
-    <t>testtest@1</t>
-  </si>
-  <si>
-    <t>test@12</t>
-  </si>
-  <si>
     <t>ABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYZ</t>
   </si>
   <si>
@@ -54,13 +57,97 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>PageTitle</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Implementation of Queue in Python</t>
+  </si>
+  <si>
+    <t>Implementation using collections.deque</t>
+  </si>
+  <si>
+    <t>Implementation using array</t>
+  </si>
+  <si>
+    <t>Queue Operations</t>
+  </si>
+  <si>
+    <t>Assessment</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Overview of Trees</t>
+  </si>
+  <si>
+    <t>Terminologies</t>
+  </si>
+  <si>
+    <t>Types of Trees</t>
+  </si>
+  <si>
+    <t>Tree Traversals</t>
+  </si>
+  <si>
+    <t>Traversals-Illustration</t>
+  </si>
+  <si>
+    <t>Binary Trees</t>
+  </si>
+  <si>
+    <t>Types of Binary Trees</t>
+  </si>
+  <si>
+    <t>Implementation in Python</t>
+  </si>
+  <si>
+    <t>Binary Tree Traversals</t>
+  </si>
+  <si>
+    <t>Implementation of Binary Trees</t>
+  </si>
+  <si>
+    <t>Applications of Binary trees</t>
+  </si>
+  <si>
+    <t>Binary Search Trees</t>
+  </si>
+  <si>
+    <t>Implementation Of BST</t>
+  </si>
+  <si>
+    <t>ValidCode</t>
+  </si>
+  <si>
+    <t>InvalidCode</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>print('Hello,World')</t>
+  </si>
+  <si>
+    <t>Hello,World</t>
+  </si>
+  <si>
+    <t>System.out.println("Hello,World");</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -76,15 +163,12 @@
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <color rgb="FF0066CC"/>
-      <name val="Courier New"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <name val="&quot;Courier New&quot;"/>
     </font>
   </fonts>
   <fills count="3">
@@ -107,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -115,19 +199,13 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -142,6 +220,18 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -375,8 +465,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="39.0"/>
-    <col customWidth="1" min="2" max="2" width="26.88"/>
-    <col customWidth="1" min="3" max="3" width="9.38"/>
+    <col customWidth="1" min="2" max="2" width="15.38"/>
+    <col customWidth="1" min="3" max="3" width="26.5"/>
     <col customWidth="1" min="4" max="4" width="15.25"/>
   </cols>
   <sheetData>
@@ -398,47 +488,43 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5"/>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -446,13 +532,10 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -460,55 +543,94 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1.23456789E8</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1.23456789E8</v>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.23456789E8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.23456789E8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -523,7 +645,217 @@
     <hyperlink r:id="rId7" ref="A8"/>
     <hyperlink r:id="rId8" ref="A9"/>
     <hyperlink r:id="rId9" ref="A10"/>
+    <hyperlink r:id="rId10" ref="A11"/>
+    <hyperlink r:id="rId11" ref="A12"/>
+    <hyperlink r:id="rId12" ref="A13"/>
   </hyperlinks>
-  <drawing r:id="rId10"/>
+  <drawing r:id="rId13"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="32.13"/>
+    <col customWidth="1" min="2" max="2" width="14.63"/>
+    <col customWidth="1" min="3" max="3" width="25.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="24.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="30.13"/>
+    <col customWidth="1" min="2" max="2" width="14.63"/>
+    <col customWidth="1" min="3" max="3" width="25.63"/>
+    <col customWidth="1" min="4" max="4" width="22.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All linked list files files
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28813"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02C2773B-0020-4C1C-9901-08583545F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{166F495F-C7CF-4C1D-9B81-7B3719CF99F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="9" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Browser" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
   <si>
     <t>Browser</t>
   </si>
@@ -244,6 +244,18 @@
   </si>
   <si>
     <t>Deletion</t>
+  </si>
+  <si>
+    <t>singly linked list</t>
+  </si>
+  <si>
+    <t>linked list</t>
+  </si>
+  <si>
+    <t>doubly linked list</t>
+  </si>
+  <si>
+    <t>type of the linked list</t>
   </si>
   <si>
     <t>Stack</t>
@@ -712,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C4823E-CFF1-4F25-B16B-5F320C2F884E}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -743,10 +755,10 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="115.5">
@@ -754,10 +766,10 @@
         <v>21</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="115.5">
@@ -765,10 +777,10 @@
         <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -777,10 +789,10 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -798,7 +810,7 @@
       <c r="B7" s="6"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="127.5">
@@ -806,11 +818,11 @@
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5">
@@ -818,11 +830,11 @@
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="104.25">
@@ -830,7 +842,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="104.25">
@@ -838,10 +850,10 @@
         <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="104.25">
@@ -849,10 +861,10 @@
         <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="104.25">
@@ -860,10 +872,10 @@
         <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1288,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430191D4-F6BD-455F-85E8-18BF3D3E4BAF}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1342,6 +1354,26 @@
     <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1369,22 +1401,22 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1410,27 +1442,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1458,22 +1490,22 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit for Q, Tree, Reg final
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -4,10 +4,15 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Browser" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Register" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Queue" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Tree" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="CodeEditor" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="SignIn" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Register" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Queue" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Tree" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="CodeEditor" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Array" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Arrays_PracticeQuestions" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Arrays_Practice_Editor" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="PythonCode" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="129">
   <si>
     <t>Browser</t>
   </si>
@@ -23,6 +28,21 @@
     <t>chrome</t>
   </si>
   <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>abc@test.com</t>
+  </si>
+  <si>
+    <t>testtest@123</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
     <t>URL</t>
   </si>
   <si>
@@ -44,7 +64,7 @@
     <t>testtest@1</t>
   </si>
   <si>
-    <t>abc@test.com</t>
+    <t>john smith</t>
   </si>
   <si>
     <t>ABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYABCDEFGHIJKLMNOPQRSTUVWXYZ</t>
@@ -56,9 +76,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>password1</t>
   </si>
   <si>
@@ -141,13 +158,315 @@
   </si>
   <si>
     <t>System.out.println("Hello,World");</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Arrays in Python</t>
+  </si>
+  <si>
+    <t>Arrays using List</t>
+  </si>
+  <si>
+    <t>Basic Operations in Lists</t>
+  </si>
+  <si>
+    <t>Applications of Array</t>
+  </si>
+  <si>
+    <t>Search The Array</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>Find Numbers with Even Numbers of Digits</t>
+  </si>
+  <si>
+    <t>Squared of a Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PageTitle </t>
+  </si>
+  <si>
+    <t>Assesment</t>
+  </si>
+  <si>
+    <t>def search(input_list, num): 
+  if(num in input_list):
+  print("Element Found")
+  else:
+  print("Not Found")
+ search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>def search(input_list, num): 
+  if(num in input_list):
+  print("Element Found")
+  else:
+  print("Element Not Found")
+ search([12, 23, 45, 67, 6, 90] , 1)</t>
+  </si>
+  <si>
+    <t>Element Not Found</t>
+  </si>
+  <si>
+    <t>Some Tests failed. Please review code</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    count = 0
+    result = 0
+    for i in range(0, len(nums)):
+        if nums[i] == 0:
+            count = 0
+        else:
+            count += 1
+        result = max(result, count)
+    print(result)
+findMaxConsecutiveOnes([1, 0, 1, 1, 0, 1])</t>
+  </si>
+  <si>
+    <t>1
+ 1
+ 2
+ 2</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+  count = 0
+  result = 0
+  for i in range(0, len(nums)):
+  if (nums[i] == 0):
+  count = 0
+  else:
+  count+= 1
+  result = max(result, count)
+  print(result)
+ findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+  c=0
+  for i in nums:
+  j=str(i)
+  x=len(j)
+  if x%2==0:
+  c=c+1
+  print(c)
+  return c</t>
+  </si>
+  <si>
+    <t>Submission Successful</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+  squares_list = []
+  for i in range(0, len(nums)):
+  square = nums[i] * nums[i];
+  squares_list.append(square)
+  sorted_squares_list = sorted(squares_list)
+  print sorted_squares_list;
+  return sorted_squares_list;
+ sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>[49]
+ [9, 49]
+ [4, 9, 49]
+ [4, 9, 9, 49]
+ [4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>No tests were collected</t>
+  </si>
+  <si>
+    <t>PythonCode</t>
+  </si>
+  <si>
+    <t>print("DSAlgo");</t>
+  </si>
+  <si>
+    <t>DSAlgo</t>
+  </si>
+  <si>
+    <t>print("NumpyNinja</t>
+  </si>
+  <si>
+    <t>NumpyNinja</t>
+  </si>
+  <si>
+    <t>grocery = ["apples", "bananas", "cucumbers", "dates", "strawberries"]</t>
+  </si>
+  <si>
+    <t>['apples', 'bananas', 'cucumbers', 'dates', 'strawberries', 'oranges']</t>
+  </si>
+  <si>
+    <t>grocery.append("oranges")</t>
+  </si>
+  <si>
+    <t>print (grocery);</t>
+  </si>
+  <si>
+    <t>NameError: name 'apples' is not defined on line 3</t>
+  </si>
+  <si>
+    <t>print[apples]</t>
+  </si>
+  <si>
+    <t>grocery = ["apples", "banana", "cucumbers", "dates","strawberries"]</t>
+  </si>
+  <si>
+    <t>['apples', 'banana', 'carrots', 'cucumbers', 'dates', 'strawberries']</t>
+  </si>
+  <si>
+    <t>grocery.insert(2, "carrots")</t>
+  </si>
+  <si>
+    <t>NameError: name 'Walnuts' is not defined on line 2</t>
+  </si>
+  <si>
+    <t>grocery.insert(10, Walnuts)</t>
+  </si>
+  <si>
+    <t>employee = ["Ann", "Ben", "Cathy", "Daisy", "Snow"]</t>
+  </si>
+  <si>
+    <t>[['Ann', 'Ben', 'Cathy', 'Daisy', 'Snow', 'Bob']]</t>
+  </si>
+  <si>
+    <t>employee.append("Bob")</t>
+  </si>
+  <si>
+    <t>print[employee]</t>
+  </si>
+  <si>
+    <t>SyntaxError: EOF in multi-line statement on line 4</t>
+  </si>
+  <si>
+    <t>print[employee</t>
+  </si>
+  <si>
+    <t>if(num in input_list):</t>
+  </si>
+  <si>
+    <t>print("Element Found")</t>
+  </si>
+  <si>
+    <t>\b</t>
+  </si>
+  <si>
+    <t>else:</t>
+  </si>
+  <si>
+    <t>print("Not Found")</t>
+  </si>
+  <si>
+    <t>search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>submission success</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :</t>
+  </si>
+  <si>
+    <t>count = 0</t>
+  </si>
+  <si>
+    <t>result = 0</t>
+  </si>
+  <si>
+    <t>for i in range(0, len(nums)):</t>
+  </si>
+  <si>
+    <t>if (nums[i] == 0):</t>
+  </si>
+  <si>
+    <t>count+= 1</t>
+  </si>
+  <si>
+    <t>result = max(result, count)</t>
+  </si>
+  <si>
+    <t>print(result)</t>
+  </si>
+  <si>
+    <t>findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):</t>
+  </si>
+  <si>
+    <t>c=0</t>
+  </si>
+  <si>
+    <t>for i in nums:</t>
+  </si>
+  <si>
+    <t>j=str(i)</t>
+  </si>
+  <si>
+    <t>x=len(j)</t>
+  </si>
+  <si>
+    <t>if x%2==0:</t>
+  </si>
+  <si>
+    <t>c=c+1</t>
+  </si>
+  <si>
+    <t>print c</t>
+  </si>
+  <si>
+    <t>return c</t>
+  </si>
+  <si>
+    <t>findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>squares_list = []</t>
+  </si>
+  <si>
+    <t>square = nums[i] * nums[i];</t>
+  </si>
+  <si>
+    <t>squares_list.append(square)</t>
+  </si>
+  <si>
+    <t>sorted_squares_list = sorted(squares_list)</t>
+  </si>
+  <si>
+    <t>print sorted_squares_list;</t>
+  </si>
+  <si>
+    <t>return sorted_squares_list;</t>
+  </si>
+  <si>
+    <t>sortedSquares([-7,-3,2,3,11])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -170,6 +489,15 @@
       <color rgb="FF0066CC"/>
       <name val="&quot;Courier New&quot;"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -191,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -207,6 +535,27 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -219,6 +568,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
@@ -232,6 +585,22 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -454,7 +823,811 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" s="11">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" s="11">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B34:B45"/>
+    <mergeCell ref="B46:B64"/>
+    <mergeCell ref="B65:B83"/>
+    <mergeCell ref="B84:B97"/>
+    <mergeCell ref="B98:B111"/>
+    <mergeCell ref="B112:B122"/>
+    <mergeCell ref="B123:B133"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B33"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -472,132 +1645,135 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
         <v>1.23456789E8</v>
@@ -608,30 +1784,30 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -653,7 +1829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -664,43 +1840,43 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="32.13"/>
-    <col customWidth="1" min="2" max="2" width="14.63"/>
+    <col customWidth="1" min="2" max="2" width="30.63"/>
     <col customWidth="1" min="3" max="3" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -708,7 +1884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -723,77 +1899,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +1977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -815,44 +1991,279 @@
     <col customWidth="1" min="2" max="2" width="14.63"/>
     <col customWidth="1" min="3" max="3" width="25.63"/>
     <col customWidth="1" min="4" max="4" width="22.75"/>
+    <col customWidth="1" min="5" max="5" width="30.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="49.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="32.88"/>
+    <col customWidth="1" min="3" max="3" width="26.63"/>
+    <col customWidth="1" min="4" max="4" width="35.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All updated files including testng files
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28814"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{166F495F-C7CF-4C1D-9B81-7B3719CF99F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1EA36D9-D706-4C9D-B61F-8BF4794FC02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="9" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Browser" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,9 @@
     <sheet name="LinkedList" sheetId="6" r:id="rId6"/>
     <sheet name="Stack" sheetId="7" r:id="rId7"/>
     <sheet name="Arrays" sheetId="8" r:id="rId8"/>
-    <sheet name="Arrays_PracticeQuestions" sheetId="9" r:id="rId9"/>
-    <sheet name="Arrays_Practice_Editor" sheetId="10" r:id="rId10"/>
+    <sheet name="Arrays_Practice_Editor" sheetId="10" r:id="rId9"/>
+    <sheet name="SignIn" sheetId="11" r:id="rId10"/>
+    <sheet name="PythonCode" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="137">
   <si>
     <t>Browser</t>
   </si>
@@ -283,18 +284,6 @@
   </si>
   <si>
     <t>Applications of Array</t>
-  </si>
-  <si>
-    <t>Search the array</t>
-  </si>
-  <si>
-    <t>Max Consecutive Ones</t>
-  </si>
-  <si>
-    <t>Find Numbers with Even Numbers of Digits</t>
-  </si>
-  <si>
-    <t>Squared of a Sorted Array</t>
   </si>
   <si>
     <t>def search(input_list, num): 
@@ -370,23 +359,207 @@
         square = nums[i] * nums[i];
         squares_list.append(square)
         sorted_squares_list = sorted(squares_list)
+    return sorted_squares_list;
+i = sortedSquares([-7,-3,2,3,11])
+print (i)</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+    squares_list = []
+    for i in range(0, len(nums)):
+        square = nums[i] * nums[i];
+        squares_list.append(square)
+        sorted_squares_list = sorted(squares_list)
         print sorted_squares_list;
     return sorted_squares_list;
 sortedSquares([-7,-3,2,3,11])</t>
   </si>
   <si>
-    <t>[49]
-[9, 49]
-[4, 9, 49]
-[4, 9, 9, 49]
-[4, 9, 9, 49, 121]</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>testtest@123</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>PythonCode</t>
+  </si>
+  <si>
+    <t>print("DSAlgo");</t>
+  </si>
+  <si>
+    <t>DSAlgo</t>
+  </si>
+  <si>
+    <t>print("NumpyNinja</t>
+  </si>
+  <si>
+    <t>NumpyNinja</t>
+  </si>
+  <si>
+    <t>grocery = ["apples", "bananas", "cucumbers", "dates", "strawberries"]</t>
+  </si>
+  <si>
+    <t>['apples', 'bananas', 'cucumbers', 'dates', 'strawberries', 'oranges']</t>
+  </si>
+  <si>
+    <t>grocery.append("oranges")</t>
+  </si>
+  <si>
+    <t>print (grocery);</t>
+  </si>
+  <si>
+    <t>NameError: name 'apples' is not defined on line 3</t>
+  </si>
+  <si>
+    <t>print[apples]</t>
+  </si>
+  <si>
+    <t>grocery = ["apples", "banana", "cucumbers", "dates","strawberries"]</t>
+  </si>
+  <si>
+    <t>['apples', 'banana', 'carrots', 'cucumbers', 'dates', 'strawberries']</t>
+  </si>
+  <si>
+    <t>grocery.insert(2, "carrots")</t>
+  </si>
+  <si>
+    <t>NameError: name 'Walnuts' is not defined on line 2</t>
+  </si>
+  <si>
+    <t>grocery.insert(10, Walnuts)</t>
+  </si>
+  <si>
+    <t>employee = ["Ann", "Ben", "Cathy", "Daisy", "Snow"]</t>
+  </si>
+  <si>
+    <t>[['Ann', 'Ben', 'Cathy', 'Daisy', 'Snow', 'Bob']]</t>
+  </si>
+  <si>
+    <t>employee.append("Bob")</t>
+  </si>
+  <si>
+    <t>print[employee]</t>
+  </si>
+  <si>
+    <t>SyntaxError: EOF in multi-line statement on line 4</t>
+  </si>
+  <si>
+    <t>print[employee</t>
+  </si>
+  <si>
+    <t>if(num in input_list):</t>
+  </si>
+  <si>
+    <t>print("Element Found")</t>
+  </si>
+  <si>
+    <t>\b</t>
+  </si>
+  <si>
+    <t>else:</t>
+  </si>
+  <si>
+    <t>print("Not Found")</t>
+  </si>
+  <si>
+    <t>search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>submission success</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :</t>
+  </si>
+  <si>
+    <t>count = 0</t>
+  </si>
+  <si>
+    <t>result = 0</t>
+  </si>
+  <si>
+    <t>for i in range(0, len(nums)):</t>
+  </si>
+  <si>
+    <t>if (nums[i] == 0):</t>
+  </si>
+  <si>
+    <t>count+= 1</t>
+  </si>
+  <si>
+    <t>result = max(result, count)</t>
+  </si>
+  <si>
+    <t>print(result)</t>
+  </si>
+  <si>
+    <t>findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):</t>
+  </si>
+  <si>
+    <t>c=0</t>
+  </si>
+  <si>
+    <t>for i in nums:</t>
+  </si>
+  <si>
+    <t>j=str(i)</t>
+  </si>
+  <si>
+    <t>x=len(j)</t>
+  </si>
+  <si>
+    <t>if x%2==0:</t>
+  </si>
+  <si>
+    <t>c=c+1</t>
+  </si>
+  <si>
+    <t>print c</t>
+  </si>
+  <si>
+    <t>return c</t>
+  </si>
+  <si>
+    <t>findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):</t>
+  </si>
+  <si>
+    <t>squares_list = []</t>
+  </si>
+  <si>
+    <t>square = nums[i] * nums[i];</t>
+  </si>
+  <si>
+    <t>squares_list.append(square)</t>
+  </si>
+  <si>
+    <t>sorted_squares_list = sorted(squares_list)</t>
+  </si>
+  <si>
+    <t>print sorted_squares_list;</t>
+  </si>
+  <si>
+    <t>return sorted_squares_list;</t>
+  </si>
+  <si>
+    <t>sortedSquares([-7,-3,2,3,11])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -412,6 +585,26 @@
       <color rgb="FF0066CC"/>
       <name val="&quot;Courier New&quot;"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -436,10 +629,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -453,8 +647,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -721,166 +921,956 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C4823E-CFF1-4F25-B16B-5F320C2F884E}">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0558F304-2491-40E5-ACF4-C8F530A5024C}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="8"/>
+      <c r="B4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="mailto:abc@test.com" xr:uid="{BA119CBF-8B9D-45F5-AD8B-F0BF4623B8D5}"/>
+    <hyperlink ref="A3" r:id="rId2" display="mailto:abc@test.com" xr:uid="{4CD662A2-A9AD-4909-A5BF-F8C7E0CBC233}"/>
+    <hyperlink ref="A5" r:id="rId3" display="mailto:abc@test.com" xr:uid="{337458B6-2388-43FD-8B9D-17A032B4E47A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD62C1B-9095-49C3-8503-21CC0ED5CAEF}">
+  <dimension ref="A1:B133"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15">
+      <c r="A1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="137.25" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="5" t="s">
+    <row r="2" spans="1:2" ht="15">
+      <c r="A2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15">
+      <c r="A3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15">
+      <c r="A4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15">
+      <c r="A5" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:2" ht="15">
+      <c r="A6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="11"/>
+    </row>
+    <row r="7" spans="1:2" ht="15">
+      <c r="A7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="11"/>
+    </row>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15">
+      <c r="A11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="1:2" ht="15">
+      <c r="A12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="11"/>
+    </row>
+    <row r="13" spans="1:2" ht="15">
+      <c r="A13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15">
+      <c r="A14" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="11"/>
+    </row>
+    <row r="15" spans="1:2" ht="15">
+      <c r="A15" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="1:2" ht="15">
+      <c r="A16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15">
+      <c r="A17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="1:2" ht="15">
+      <c r="A18" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:2" ht="15">
+      <c r="A19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15">
+      <c r="A20" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="1:2" ht="15">
+      <c r="A21" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:2" ht="15">
+      <c r="A22" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="115.5">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="115.5">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="127.5">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="5" t="s">
+      <c r="B22" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15">
+      <c r="A23" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="11"/>
+    </row>
+    <row r="24" spans="1:2" ht="15">
+      <c r="A24" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="1:2" ht="15">
+      <c r="A25" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:2" ht="15">
+      <c r="A26" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="11"/>
+    </row>
+    <row r="27" spans="1:2" ht="15">
+      <c r="A27" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" spans="1:2" ht="15">
+      <c r="A28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" spans="1:2" ht="15">
+      <c r="A29" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="11"/>
+    </row>
+    <row r="30" spans="1:2" ht="15">
+      <c r="A30" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="1:2" ht="15">
+      <c r="A31" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" spans="1:2" ht="15">
+      <c r="A32" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="1:2" ht="15">
+      <c r="A33" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:2" ht="15">
+      <c r="A34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15">
+      <c r="A35" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" spans="1:2" ht="15">
+      <c r="A36" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="11"/>
+    </row>
+    <row r="37" spans="1:2" ht="15">
+      <c r="A37" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="11"/>
+    </row>
+    <row r="38" spans="1:2" ht="15">
+      <c r="A38" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="11"/>
+    </row>
+    <row r="39" spans="1:2" ht="15">
+      <c r="A39" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="11"/>
+    </row>
+    <row r="40" spans="1:2" ht="15">
+      <c r="A40" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="11"/>
+    </row>
+    <row r="41" spans="1:2" ht="15">
+      <c r="A41" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="11"/>
+    </row>
+    <row r="42" spans="1:2" ht="15">
+      <c r="A42" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" s="11"/>
+    </row>
+    <row r="43" spans="1:2" ht="15">
+      <c r="A43" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="11"/>
+    </row>
+    <row r="44" spans="1:2" ht="15">
+      <c r="A44" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="11"/>
+    </row>
+    <row r="45" spans="1:2" ht="15">
+      <c r="A45" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="11"/>
+    </row>
+    <row r="46" spans="1:2" ht="15">
+      <c r="A46" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15">
+      <c r="A47" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="11"/>
+    </row>
+    <row r="48" spans="1:2" ht="15">
+      <c r="A48" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" s="11"/>
+    </row>
+    <row r="49" spans="1:2" ht="15">
+      <c r="A49" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="11"/>
+    </row>
+    <row r="50" spans="1:2" ht="15">
+      <c r="A50" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="11"/>
+    </row>
+    <row r="51" spans="1:2" ht="15">
+      <c r="A51" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="11"/>
+    </row>
+    <row r="52" spans="1:2" ht="15">
+      <c r="A52" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="11"/>
+    </row>
+    <row r="53" spans="1:2" ht="15">
+      <c r="A53" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="11"/>
+    </row>
+    <row r="54" spans="1:2" ht="15">
+      <c r="A54" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="11"/>
+    </row>
+    <row r="55" spans="1:2" ht="15">
+      <c r="A55" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="11"/>
+    </row>
+    <row r="56" spans="1:2" ht="15">
+      <c r="A56" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="11"/>
+    </row>
+    <row r="57" spans="1:2" ht="15">
+      <c r="A57" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" s="11"/>
+    </row>
+    <row r="58" spans="1:2" ht="15">
+      <c r="A58" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="11"/>
+    </row>
+    <row r="59" spans="1:2" ht="15">
+      <c r="A59" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="11"/>
+    </row>
+    <row r="60" spans="1:2" ht="15">
+      <c r="A60" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" s="11"/>
+    </row>
+    <row r="61" spans="1:2" ht="15">
+      <c r="A61" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="11"/>
+    </row>
+    <row r="62" spans="1:2" ht="15">
+      <c r="A62" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="11"/>
+    </row>
+    <row r="63" spans="1:2" ht="15">
+      <c r="A63" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="11"/>
+    </row>
+    <row r="64" spans="1:2" ht="15">
+      <c r="A64" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" s="11"/>
+    </row>
+    <row r="65" spans="1:2" ht="15">
+      <c r="A65" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15">
+      <c r="A66" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="11"/>
+    </row>
+    <row r="67" spans="1:2" ht="15">
+      <c r="A67" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="11"/>
+    </row>
+    <row r="68" spans="1:2" ht="15">
+      <c r="A68" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="11"/>
+    </row>
+    <row r="69" spans="1:2" ht="15">
+      <c r="A69" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B69" s="11"/>
+    </row>
+    <row r="70" spans="1:2" ht="15">
+      <c r="A70" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="11"/>
+    </row>
+    <row r="71" spans="1:2" ht="15">
+      <c r="A71" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" s="11"/>
+    </row>
+    <row r="72" spans="1:2" ht="15">
+      <c r="A72" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B72" s="11"/>
+    </row>
+    <row r="73" spans="1:2" ht="15">
+      <c r="A73" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B73" s="11"/>
+    </row>
+    <row r="74" spans="1:2" ht="15">
+      <c r="A74" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B74" s="11"/>
+    </row>
+    <row r="75" spans="1:2" ht="15">
+      <c r="A75" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B75" s="11"/>
+    </row>
+    <row r="76" spans="1:2" ht="15">
+      <c r="A76" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B76" s="11"/>
+    </row>
+    <row r="77" spans="1:2" ht="15">
+      <c r="A77" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B77" s="11"/>
+    </row>
+    <row r="78" spans="1:2" ht="15">
+      <c r="A78" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" s="11"/>
+    </row>
+    <row r="79" spans="1:2" ht="15">
+      <c r="A79" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B79" s="11"/>
+    </row>
+    <row r="80" spans="1:2" ht="15">
+      <c r="A80" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B80" s="11"/>
+    </row>
+    <row r="81" spans="1:2" ht="15">
+      <c r="A81" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B81" s="11"/>
+    </row>
+    <row r="82" spans="1:2" ht="15">
+      <c r="A82" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B82" s="11"/>
+    </row>
+    <row r="83" spans="1:2" ht="15">
+      <c r="A83" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B83" s="11"/>
+    </row>
+    <row r="84" spans="1:2" ht="15">
+      <c r="A84" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B84" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15">
+      <c r="A85" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B85" s="11"/>
+    </row>
+    <row r="86" spans="1:2" ht="15">
+      <c r="A86" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B86" s="11"/>
+    </row>
+    <row r="87" spans="1:2" ht="15">
+      <c r="A87" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B87" s="11"/>
+    </row>
+    <row r="88" spans="1:2" ht="15">
+      <c r="A88" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B88" s="11"/>
+    </row>
+    <row r="89" spans="1:2" ht="15">
+      <c r="A89" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B89" s="11"/>
+    </row>
+    <row r="90" spans="1:2" ht="15">
+      <c r="A90" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B90" s="11"/>
+    </row>
+    <row r="91" spans="1:2" ht="15">
+      <c r="A91" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B91" s="11"/>
+    </row>
+    <row r="92" spans="1:2" ht="15">
+      <c r="A92" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92" s="11"/>
+    </row>
+    <row r="93" spans="1:2" ht="15">
+      <c r="A93" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B93" s="11"/>
+    </row>
+    <row r="94" spans="1:2" ht="15">
+      <c r="A94" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94" s="11"/>
+    </row>
+    <row r="95" spans="1:2" ht="15">
+      <c r="A95" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B95" s="11"/>
+    </row>
+    <row r="96" spans="1:2" ht="15">
+      <c r="A96" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B96" s="11"/>
+    </row>
+    <row r="97" spans="1:2" ht="15">
+      <c r="A97" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B97" s="11"/>
+    </row>
+    <row r="98" spans="1:2" ht="15">
+      <c r="A98" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15">
+      <c r="A99" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B99" s="11"/>
+    </row>
+    <row r="100" spans="1:2" ht="15">
+      <c r="A100" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B100" s="11"/>
+    </row>
+    <row r="101" spans="1:2" ht="15">
+      <c r="A101" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B101" s="11"/>
+    </row>
+    <row r="102" spans="1:2" ht="15">
+      <c r="A102" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B102" s="11"/>
+    </row>
+    <row r="103" spans="1:2" ht="15">
+      <c r="A103" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B103" s="11"/>
+    </row>
+    <row r="104" spans="1:2" ht="15">
+      <c r="A104" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B104" s="11"/>
+    </row>
+    <row r="105" spans="1:2" ht="15">
+      <c r="A105" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" s="11"/>
+    </row>
+    <row r="106" spans="1:2" ht="15">
+      <c r="A106" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" s="11"/>
+    </row>
+    <row r="107" spans="1:2" ht="15">
+      <c r="A107" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B107" s="11"/>
+    </row>
+    <row r="108" spans="1:2" ht="15">
+      <c r="A108" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B108" s="11"/>
+    </row>
+    <row r="109" spans="1:2" ht="15">
+      <c r="A109" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B109" s="11"/>
+    </row>
+    <row r="110" spans="1:2" ht="15">
+      <c r="A110" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B110" s="11"/>
+    </row>
+    <row r="111" spans="1:2" ht="15">
+      <c r="A111" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B111" s="11"/>
+    </row>
+    <row r="112" spans="1:2" ht="15">
+      <c r="A112" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B112" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="127.5">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="104.25">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="104.25">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="104.25">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="104.25">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" t="s">
-        <v>71</v>
-      </c>
+    <row r="113" spans="1:2" ht="15">
+      <c r="A113" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B113" s="11"/>
+    </row>
+    <row r="114" spans="1:2" ht="15">
+      <c r="A114" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114" s="11"/>
+    </row>
+    <row r="115" spans="1:2" ht="15">
+      <c r="A115" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B115" s="11"/>
+    </row>
+    <row r="116" spans="1:2" ht="15">
+      <c r="A116" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B116" s="11"/>
+    </row>
+    <row r="117" spans="1:2" ht="15">
+      <c r="A117" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B117" s="11"/>
+    </row>
+    <row r="118" spans="1:2" ht="15">
+      <c r="A118" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B118" s="11"/>
+    </row>
+    <row r="119" spans="1:2" ht="15">
+      <c r="A119" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B119" s="11"/>
+    </row>
+    <row r="120" spans="1:2" ht="15">
+      <c r="A120" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B120" s="11"/>
+    </row>
+    <row r="121" spans="1:2" ht="15">
+      <c r="A121" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B121" s="11"/>
+    </row>
+    <row r="122" spans="1:2" ht="15">
+      <c r="A122" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B122" s="11"/>
+    </row>
+    <row r="123" spans="1:2" ht="15">
+      <c r="A123" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15">
+      <c r="A124" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B124" s="11"/>
+    </row>
+    <row r="125" spans="1:2" ht="15">
+      <c r="A125" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B125" s="11"/>
+    </row>
+    <row r="126" spans="1:2" ht="15">
+      <c r="A126" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B126" s="11"/>
+    </row>
+    <row r="127" spans="1:2" ht="15">
+      <c r="A127" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B127" s="11"/>
+    </row>
+    <row r="128" spans="1:2" ht="15">
+      <c r="A128" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B128" s="11"/>
+    </row>
+    <row r="129" spans="1:2" ht="15">
+      <c r="A129" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B129" s="11"/>
+    </row>
+    <row r="130" spans="1:2" ht="15">
+      <c r="A130" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B130" s="11"/>
+    </row>
+    <row r="131" spans="1:2" ht="15">
+      <c r="A131" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B131" s="11"/>
+    </row>
+    <row r="132" spans="1:2" ht="15">
+      <c r="A132" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B132" s="11"/>
+    </row>
+    <row r="133" spans="1:2" ht="15">
+      <c r="A133" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B133" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B112:B122"/>
+    <mergeCell ref="B123:B133"/>
+    <mergeCell ref="B22:B33"/>
+    <mergeCell ref="B34:B45"/>
+    <mergeCell ref="B46:B64"/>
+    <mergeCell ref="B65:B83"/>
+    <mergeCell ref="B84:B97"/>
+    <mergeCell ref="B98:B111"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1302,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430191D4-F6BD-455F-85E8-18BF3D3E4BAF}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1471,44 +2461,165 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFEF127-E918-4D11-9C4A-03C0FEC05F86}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C4823E-CFF1-4F25-B16B-5F320C2F884E}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="137.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="D2" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="3" spans="1:4" ht="115.5">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="D3" s="1" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="115.5">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="127.5">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="127.5">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="104.25">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="104.25">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="115.5">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="104.25">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated POM, TestData, Corrected Duplicates
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -9,7 +9,7 @@
     <sheet state="visible" name="Queue" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Tree" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="CodeEditor" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Array" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Arrays" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Arrays_PracticeQuestions" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Arrays_Practice_Editor" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="PythonCode" sheetId="10" r:id="rId13"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="129">
   <si>
     <t>Browser</t>
   </si>
@@ -508,8 +508,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE8F2FE"/>
-        <bgColor rgb="FFE8F2FE"/>
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,12 +519,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -532,7 +535,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -834,718 +837,718 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="11" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B46" s="11">
+      <c r="B46" s="12">
         <v>2.0</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="11" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="11" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="11" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="11" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="10" t="s">
+      <c r="A61" s="11" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="11" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="11" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="11" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="11" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="10" t="s">
+      <c r="A77" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="10" t="s">
+      <c r="A79" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="10" t="s">
+      <c r="A80" s="11" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="10" t="s">
+      <c r="A81" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="10" t="s">
+      <c r="A82" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="10" t="s">
+      <c r="A83" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="10" t="s">
+      <c r="A84" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B84" s="11">
+      <c r="B84" s="12">
         <v>2.0</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="10" t="s">
+      <c r="A87" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="10" t="s">
+      <c r="A88" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="10" t="s">
+      <c r="A89" s="11" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="11" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="10" t="s">
+      <c r="A91" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="10" t="s">
+      <c r="A93" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="10" t="s">
+      <c r="A94" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="10" t="s">
+      <c r="A95" s="11" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="10" t="s">
+      <c r="A96" s="11" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="10" t="s">
+      <c r="A97" s="11" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B98" s="10" t="s">
+      <c r="B98" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="10" t="s">
+      <c r="A99" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="10" t="s">
+      <c r="A100" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="10" t="s">
+      <c r="A101" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="10" t="s">
+      <c r="A102" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="10" t="s">
+      <c r="A103" s="11" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="10" t="s">
+      <c r="A104" s="11" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="10" t="s">
+      <c r="A105" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="10" t="s">
+      <c r="A106" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="10" t="s">
+      <c r="A108" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="10" t="s">
+      <c r="A109" s="11" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="10" t="s">
+      <c r="A110" s="11" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="10" t="s">
+      <c r="A111" s="11" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="10" t="s">
+      <c r="A112" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="B112" s="11" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="10" t="s">
+      <c r="A113" s="11" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="10" t="s">
+      <c r="A114" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="10" t="s">
+      <c r="A115" s="11" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="10" t="s">
+      <c r="A116" s="11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="10" t="s">
+      <c r="A117" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="10" t="s">
+      <c r="A118" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="10" t="s">
+      <c r="A119" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="10" t="s">
+      <c r="A120" s="11" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="10" t="s">
+      <c r="A121" s="11" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="10" t="s">
+      <c r="A122" s="11" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="10" t="s">
+      <c r="A123" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B123" s="10" t="s">
+      <c r="B123" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="10" t="s">
+      <c r="A124" s="11" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="10" t="s">
+      <c r="A125" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="10" t="s">
+      <c r="A126" s="11" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="10" t="s">
+      <c r="A128" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="10" t="s">
+      <c r="A129" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="10" t="s">
+      <c r="A130" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="10" t="s">
+      <c r="A131" s="11" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="10" t="s">
+      <c r="A132" s="11" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="10" t="s">
+      <c r="A133" s="11" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1647,18 +1650,18 @@
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1672,17 +1675,13 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1691,9 +1690,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1705,9 +1702,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1716,9 +1711,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A7" s="5"/>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1727,9 +1720,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1741,9 +1732,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1755,9 +1744,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="5"/>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1769,9 +1756,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1783,9 +1768,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A12" s="5"/>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1797,9 +1780,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A13" s="5"/>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1813,19 +1794,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A5"/>
-    <hyperlink r:id="rId5" ref="A6"/>
-    <hyperlink r:id="rId6" ref="A7"/>
-    <hyperlink r:id="rId7" ref="A8"/>
-    <hyperlink r:id="rId8" ref="A9"/>
-    <hyperlink r:id="rId9" ref="A10"/>
-    <hyperlink r:id="rId10" ref="A11"/>
-    <hyperlink r:id="rId11" ref="A12"/>
-    <hyperlink r:id="rId12" ref="A13"/>
   </hyperlinks>
-  <drawing r:id="rId13"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2012,7 +1982,7 @@
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -2159,11 +2129,11 @@
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2171,11 +2141,11 @@
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2183,11 +2153,11 @@
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2195,11 +2165,11 @@
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>63</v>
       </c>
       <c r="F5" s="1">
@@ -2210,11 +2180,11 @@
       <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2222,11 +2192,11 @@
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2234,11 +2204,11 @@
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="9" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2246,11 +2216,11 @@
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2258,11 +2228,11 @@
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="9" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
madhavi files with test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajitha/DsAlgo/DSAlgo_March2025/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C549AF40-C8B7-4ED6-A9EA-D9EE3B029659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CF578D5-C94C-4D41-937E-501652ED03B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23060" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23060" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Browser" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
     <t>Error occurred during submission</t>
   </si>
   <si>
-    <t>" No tests were collected</t>
+    <t xml:space="preserve"> No tests were collected</t>
   </si>
   <si>
     <t>def findMaxConsecutiveOnes(nums) :
@@ -615,12 +615,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,47 +864,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DCABC4-BCC9-432D-ADC9-663D639FBD68}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="10" t="s">
         <v>65</v>
       </c>
     </row>
@@ -977,7 +977,7 @@
       <c r="A4" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>77</v>
       </c>
     </row>
@@ -985,19 +985,19 @@
       <c r="A5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="12"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="12"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1005,19 +1005,19 @@
       <c r="A8" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1025,19 +1025,19 @@
       <c r="A11" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="12"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1045,19 +1045,19 @@
       <c r="A14" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="12"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="12"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1065,19 +1065,19 @@
       <c r="A17" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="12"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="12"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1085,19 +1085,19 @@
       <c r="A20" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="11"/>
+      <c r="B20" s="12"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="12"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1105,73 +1105,73 @@
       <c r="A23" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="11"/>
+      <c r="B23" s="12"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="11"/>
+      <c r="B24" s="12"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="11"/>
+      <c r="B25" s="12"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="11"/>
+      <c r="B26" s="12"/>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="11"/>
+      <c r="B27" s="12"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="11"/>
+      <c r="B28" s="12"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="11"/>
+      <c r="B29" s="12"/>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="11"/>
+      <c r="B30" s="12"/>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="11"/>
+      <c r="B31" s="12"/>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="11"/>
+      <c r="B32" s="12"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="11"/>
+      <c r="B33" s="12"/>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="11" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1179,73 +1179,73 @@
       <c r="A35" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="11"/>
+      <c r="B35" s="12"/>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="11"/>
+      <c r="B36" s="12"/>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="11"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="11"/>
+      <c r="B38" s="12"/>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="11"/>
+      <c r="B39" s="12"/>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B40" s="11"/>
+      <c r="B40" s="12"/>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="11"/>
+      <c r="B41" s="12"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="11"/>
+      <c r="B42" s="12"/>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="11"/>
+      <c r="B43" s="12"/>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B44" s="11"/>
+      <c r="B44" s="12"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B45" s="11"/>
+      <c r="B45" s="12"/>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="12">
+      <c r="B46" s="13">
         <v>2</v>
       </c>
     </row>
@@ -1253,115 +1253,115 @@
       <c r="A47" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B47" s="11"/>
+      <c r="B47" s="12"/>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B48" s="11"/>
+      <c r="B48" s="12"/>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="11"/>
+      <c r="B49" s="12"/>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="11"/>
+      <c r="B50" s="12"/>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B51" s="11"/>
+      <c r="B51" s="12"/>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="11"/>
+      <c r="B52" s="12"/>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="11"/>
+      <c r="B53" s="12"/>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="11"/>
+      <c r="B54" s="12"/>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="11"/>
+      <c r="B55" s="12"/>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B56" s="11"/>
+      <c r="B56" s="12"/>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="11"/>
+      <c r="B57" s="12"/>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B58" s="11"/>
+      <c r="B58" s="12"/>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B59" s="11"/>
+      <c r="B59" s="12"/>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="11"/>
+      <c r="B60" s="12"/>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B61" s="11"/>
+      <c r="B61" s="12"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="11"/>
+      <c r="B62" s="12"/>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B63" s="11"/>
+      <c r="B63" s="12"/>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B64" s="11"/>
+      <c r="B64" s="12"/>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="11" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1369,115 +1369,115 @@
       <c r="A66" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B66" s="11"/>
+      <c r="B66" s="12"/>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B67" s="11"/>
+      <c r="B67" s="12"/>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B68" s="11"/>
+      <c r="B68" s="12"/>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B69" s="11"/>
+      <c r="B69" s="12"/>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B70" s="11"/>
+      <c r="B70" s="12"/>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B71" s="11"/>
+      <c r="B71" s="12"/>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B72" s="11"/>
+      <c r="B72" s="12"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B73" s="11"/>
+      <c r="B73" s="12"/>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B74" s="11"/>
+      <c r="B74" s="12"/>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B75" s="11"/>
+      <c r="B75" s="12"/>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B76" s="11"/>
+      <c r="B76" s="12"/>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B77" s="11"/>
+      <c r="B77" s="12"/>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B78" s="11"/>
+      <c r="B78" s="12"/>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B79" s="11"/>
+      <c r="B79" s="12"/>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B80" s="11"/>
+      <c r="B80" s="12"/>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B81" s="11"/>
+      <c r="B81" s="12"/>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B82" s="11"/>
+      <c r="B82" s="12"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B83" s="11"/>
+      <c r="B83" s="12"/>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B84" s="12">
+      <c r="B84" s="13">
         <v>2</v>
       </c>
     </row>
@@ -1485,85 +1485,85 @@
       <c r="A85" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B85" s="11"/>
+      <c r="B85" s="12"/>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B86" s="11"/>
+      <c r="B86" s="12"/>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B87" s="11"/>
+      <c r="B87" s="12"/>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B88" s="11"/>
+      <c r="B88" s="12"/>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B89" s="11"/>
+      <c r="B89" s="12"/>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B90" s="11"/>
+      <c r="B90" s="12"/>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B91" s="11"/>
+      <c r="B91" s="12"/>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B92" s="11"/>
+      <c r="B92" s="12"/>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B93" s="11"/>
+      <c r="B93" s="12"/>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B94" s="11"/>
+      <c r="B94" s="12"/>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B95" s="11"/>
+      <c r="B95" s="12"/>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B96" s="11"/>
+      <c r="B96" s="12"/>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B97" s="11"/>
+      <c r="B97" s="12"/>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B98" s="10" t="s">
+      <c r="B98" s="11" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1571,85 +1571,85 @@
       <c r="A99" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B99" s="11"/>
+      <c r="B99" s="12"/>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B100" s="11"/>
+      <c r="B100" s="12"/>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B101" s="11"/>
+      <c r="B101" s="12"/>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B102" s="11"/>
+      <c r="B102" s="12"/>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B103" s="11"/>
+      <c r="B103" s="12"/>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B104" s="11"/>
+      <c r="B104" s="12"/>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B105" s="11"/>
+      <c r="B105" s="12"/>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B106" s="11"/>
+      <c r="B106" s="12"/>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B107" s="11"/>
+      <c r="B107" s="12"/>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B108" s="11"/>
+      <c r="B108" s="12"/>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B109" s="11"/>
+      <c r="B109" s="12"/>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B110" s="11"/>
+      <c r="B110" s="12"/>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B111" s="11"/>
+      <c r="B111" s="12"/>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="B112" s="11" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1657,67 +1657,67 @@
       <c r="A113" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B113" s="11"/>
+      <c r="B113" s="12"/>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B114" s="11"/>
+      <c r="B114" s="12"/>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B115" s="11"/>
+      <c r="B115" s="12"/>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B116" s="11"/>
+      <c r="B116" s="12"/>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B117" s="11"/>
+      <c r="B117" s="12"/>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B118" s="11"/>
+      <c r="B118" s="12"/>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B119" s="11"/>
+      <c r="B119" s="12"/>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B120" s="11"/>
+      <c r="B120" s="12"/>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B121" s="11"/>
+      <c r="B121" s="12"/>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B122" s="11"/>
+      <c r="B122" s="12"/>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B123" s="10" t="s">
+      <c r="B123" s="11" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1725,61 +1725,61 @@
       <c r="A124" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B124" s="11"/>
+      <c r="B124" s="12"/>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B125" s="11"/>
+      <c r="B125" s="12"/>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B126" s="11"/>
+      <c r="B126" s="12"/>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B127" s="11"/>
+      <c r="B127" s="12"/>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B128" s="11"/>
+      <c r="B128" s="12"/>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B129" s="11"/>
+      <c r="B129" s="12"/>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B130" s="11"/>
+      <c r="B130" s="12"/>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B131" s="11"/>
+      <c r="B131" s="12"/>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B132" s="11"/>
+      <c r="B132" s="12"/>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B133" s="11"/>
+      <c r="B133" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1806,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB8416B-9243-4581-8EBF-1BB7D0382C41}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>